<commit_message>
agrid and css refactory
</commit_message>
<xml_diff>
--- a/frontend/data/clari_sample.xlsx
+++ b/frontend/data/clari_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jongb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Streamlit_UI\frontend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8AA015-7903-4EB3-9661-85127D7DED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF620EE-3F4F-4F96-9B98-FE5CC20504BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="11520" xr2:uid="{5D95BF84-7D5E-4F79-90AF-F2B5BE510451}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5D95BF84-7D5E-4F79-90AF-F2B5BE510451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>D:/Streamlit_UI/frontend/static/images/FWG.pdf</t>
+  </si>
+  <si>
+    <t>D:/Streamlit_UI/frontend/static/images/Traditional_RAG_Workflow_naive.gif</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,7 +517,7 @@
     <row r="2" spans="1:9" ht="45">
       <c r="A2" s="3">
         <f t="shared" ref="A2:A7" ca="1" si="0">RANDBETWEEN(10000, 20000)</f>
-        <v>11869</v>
+        <v>14653</v>
       </c>
       <c r="B2" s="3">
         <v>8000</v>
@@ -542,7 +545,7 @@
     <row r="3" spans="1:9" ht="60">
       <c r="A3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>11539</v>
+        <v>18161</v>
       </c>
       <c r="B3" s="3">
         <v>8000</v>
@@ -568,7 +571,7 @@
     <row r="4" spans="1:9" ht="45">
       <c r="A4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>17041</v>
+        <v>16573</v>
       </c>
       <c r="B4" s="3">
         <v>8000</v>
@@ -589,11 +592,14 @@
         <v>3000</v>
       </c>
       <c r="H4" s="3"/>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="45">
       <c r="A5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>10918</v>
+        <v>12293</v>
       </c>
       <c r="B5" s="3">
         <v>9002</v>
@@ -616,7 +622,7 @@
     <row r="6" spans="1:9" ht="45">
       <c r="A6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>18597</v>
+        <v>14570</v>
       </c>
       <c r="B6" s="3">
         <v>9002</v>
@@ -641,7 +647,7 @@
     <row r="7" spans="1:9" ht="60">
       <c r="A7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>10360</v>
+        <v>14110</v>
       </c>
       <c r="B7" s="3">
         <v>9002</v>

</xml_diff>